<commit_message>
tested correlation between yield and TT
</commit_message>
<xml_diff>
--- a/correlation_temp.xlsx
+++ b/correlation_temp.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s2096910_ed_ac_uk/Documents/dissertation/dissertation/dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{DE492314-AD92-B149-AA3E-3183B2B4EF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="14_{DE492314-AD92-B149-AA3E-3183B2B4EF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CC58711-25FF-D14B-B986-86FA5956C920}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="620" windowWidth="27240" windowHeight="15440"/>
+    <workbookView xWindow="1560" yWindow="620" windowWidth="27240" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="correlation_temp" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>year</t>
   </si>
@@ -59,12 +59,15 @@
   </si>
   <si>
     <t>X4</t>
+  </si>
+  <si>
+    <t>av_yield</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -550,10 +553,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -593,7 +597,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="42"/>
+    <cellStyle name="Normal 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -909,16 +913,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -934,8 +941,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -951,8 +961,11 @@
       <c r="E2">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="3">
+        <v>0.17721325648415001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -968,8 +981,11 @@
       <c r="E3">
         <v>-0.26</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="3">
+        <v>0.22910562474155199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -985,8 +1001,11 @@
       <c r="E4">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="3">
+        <v>0.29631972789115602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1002,8 +1021,11 @@
       <c r="E5">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="3">
+        <v>0.42959006211180101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1019,8 +1041,11 @@
       <c r="E6">
         <v>1.44</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="2">
+        <v>0.32074796</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1036,8 +1061,11 @@
       <c r="E7">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="2">
+        <v>0.31828000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1053,8 +1081,11 @@
       <c r="E8">
         <v>2.37</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="2">
+        <v>0.29363772999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1070,8 +1101,11 @@
       <c r="E9">
         <v>2.08</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="2">
+        <v>0.35416789999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1087,8 +1121,11 @@
       <c r="E10">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="3">
+        <v>0.42882083958021</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1104,8 +1141,11 @@
       <c r="E11">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="3">
+        <v>0.43623343848580398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1121,8 +1161,11 @@
       <c r="E12">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="3">
+        <v>0.52731924360400395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1138,8 +1181,11 @@
       <c r="E13">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="3">
+        <v>0.43606736842105298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1155,8 +1201,11 @@
       <c r="E14">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="2">
+        <v>0.31879613000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1172,8 +1221,11 @@
       <c r="E15">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="2">
+        <v>0.25498253999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1189,8 +1241,11 @@
       <c r="E16">
         <v>1.39</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="2">
+        <v>0.38301719000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1205,6 +1260,9 @@
       </c>
       <c r="E17">
         <v>0.53</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.28152530999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>